<commit_message>
reverted to correct 2018 data
</commit_message>
<xml_diff>
--- a/static/download/2017/RP2_SAF_JC_2017.xlsx
+++ b/static/download/2017/RP2_SAF_JC_2017.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="103">
   <si>
     <t>Number of Questions Answered with Y/N</t>
   </si>
@@ -34,24 +34,30 @@
     <t>1.0</t>
   </si>
   <si>
+    <t>Release date</t>
+  </si>
+  <si>
+    <t>Meta data</t>
+  </si>
+  <si>
     <t>Legal/Judiciary</t>
   </si>
   <si>
     <t>Occurences</t>
   </si>
   <si>
-    <t>Release date</t>
-  </si>
-  <si>
     <t>YEAR</t>
   </si>
   <si>
-    <t>Meta data</t>
+    <t>Contact</t>
   </si>
   <si>
     <t>FAB</t>
   </si>
   <si>
+    <t>ANSP</t>
+  </si>
+  <si>
     <t>State</t>
   </si>
   <si>
@@ -61,15 +67,9 @@
     <t>No</t>
   </si>
   <si>
-    <t>ANSP</t>
-  </si>
-  <si>
     <t>Baltic FAB</t>
   </si>
   <si>
-    <t>Contact</t>
-  </si>
-  <si>
     <t>ORO NAVIGACIJA</t>
   </si>
   <si>
@@ -79,22 +79,28 @@
     <t>PANSA</t>
   </si>
   <si>
+    <t>Poland</t>
+  </si>
+  <si>
     <t>BLUE MED FAB</t>
   </si>
   <si>
     <t>CYATS</t>
   </si>
   <si>
-    <t>Poland</t>
+    <t>Cyprus</t>
   </si>
   <si>
     <t>ENAV</t>
   </si>
   <si>
+    <t>Greece</t>
+  </si>
+  <si>
     <t>HANSP</t>
   </si>
   <si>
-    <t>Cyprus</t>
+    <t>Italy</t>
   </si>
   <si>
     <t>MATS</t>
@@ -106,34 +112,37 @@
     <t>BULATSA</t>
   </si>
   <si>
-    <t>Greece</t>
-  </si>
-  <si>
     <t>ROMATSA</t>
   </si>
   <si>
+    <t>Malta</t>
+  </si>
+  <si>
     <t>DK-SE FAB</t>
   </si>
   <si>
     <t>NAVIAIR</t>
   </si>
   <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
     <t>LFV</t>
   </si>
   <si>
-    <t>Italy</t>
+    <t>Romania</t>
   </si>
   <si>
     <t>2017</t>
   </si>
   <si>
-    <t>Malta</t>
+    <t>Denmark</t>
   </si>
   <si>
     <t>FAB CE</t>
   </si>
   <si>
-    <t>Bulgaria</t>
+    <t>Sweden</t>
   </si>
   <si>
     <t>ANS CR</t>
@@ -142,42 +151,33 @@
     <t>13</t>
   </si>
   <si>
-    <t>Romania</t>
-  </si>
-  <si>
-    <t>Denmark</t>
-  </si>
-  <si>
-    <t>Sweden</t>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>1</t>
+    <t>6</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
-    <t>Austria</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>6</t>
+    <t>Czech Republic</t>
   </si>
   <si>
     <t>Austro Control</t>
   </si>
   <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
     <t>Hungary</t>
   </si>
   <si>
@@ -196,36 +196,39 @@
     <t>Slovenia Control</t>
   </si>
   <si>
+    <t>FABEC</t>
+  </si>
+  <si>
+    <t>ANA LUX</t>
+  </si>
+  <si>
     <t>Slovenia</t>
   </si>
   <si>
-    <t>FABEC</t>
-  </si>
-  <si>
-    <t>ANA LUX</t>
+    <t>Belgocontrol</t>
   </si>
   <si>
     <t>Croatia</t>
   </si>
   <si>
-    <t>Belgocontrol</t>
-  </si>
-  <si>
     <t>Belgium</t>
   </si>
   <si>
+    <t>France</t>
+  </si>
+  <si>
     <t>DFS</t>
   </si>
   <si>
-    <t>France</t>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Change date</t>
   </si>
   <si>
     <t>DSNA</t>
   </si>
   <si>
-    <t>Germany</t>
-  </si>
-  <si>
     <t>Luxembourg</t>
   </si>
   <si>
@@ -241,39 +244,51 @@
     <t>Switzerland</t>
   </si>
   <si>
+    <t>SKYGUIDE</t>
+  </si>
+  <si>
     <t>NEFAB</t>
   </si>
   <si>
     <t>Estonia</t>
   </si>
   <si>
+    <t>Entity</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
+    <t>Avinor</t>
+  </si>
+  <si>
     <t>Finland</t>
   </si>
   <si>
-    <t>SKYGUIDE</t>
+    <t>EANS</t>
   </si>
   <si>
     <t>Latvia</t>
   </si>
   <si>
-    <t>Avinor</t>
-  </si>
-  <si>
-    <t>EANS</t>
-  </si>
-  <si>
     <t>ANS Finland</t>
   </si>
   <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
     <t>Norway</t>
   </si>
   <si>
+    <t>ALL</t>
+  </si>
+  <si>
     <t>SW FAB</t>
   </si>
   <si>
@@ -283,40 +298,31 @@
     <t>Spain</t>
   </si>
   <si>
+    <t>LGS</t>
+  </si>
+  <si>
     <t>UK-Ireland FAB</t>
   </si>
   <si>
     <t>Ireland</t>
   </si>
   <si>
-    <t>LGS</t>
+    <t>ENAIRE</t>
   </si>
   <si>
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>ENAIRE</t>
-  </si>
-  <si>
-    <t>Change date</t>
-  </si>
-  <si>
     <t>NAV Portugal</t>
   </si>
   <si>
+    <t>Updated with latest information from EASA</t>
+  </si>
+  <si>
     <t>IAA</t>
   </si>
   <si>
     <t>NATS NERL</t>
-  </si>
-  <si>
-    <t>Entity</t>
-  </si>
-  <si>
-    <t>Period</t>
-  </si>
-  <si>
-    <t>Comment</t>
   </si>
 </sst>
 </file>
@@ -326,7 +332,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -343,11 +349,16 @@
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF396EA2"/>
+      <name val="Calibri"/>
+    </font>
     <font/>
     <font>
       <sz val="9.0"/>
       <color rgb="FF396EA2"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -356,13 +367,18 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10.0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <sz val="9.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="9.0"/>
@@ -462,48 +478,48 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -519,28 +535,37 @@
     <xf borderId="0" fillId="5" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="4" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="4" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="2" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -581,43 +606,43 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="10">
-        <v>43195.0</v>
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="9">
+        <v>43311.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="14" t="str">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="12" t="str">
         <f>HYPERLINK("http://prudata.webfactional.com/wiki/index.php/Reporting_of_Just_Culture","Reporting of Just Culture")</f>
         <v>Reporting of Just Culture</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="14" t="str">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="12" t="str">
         <f>HYPERLINK("mailto:NSA-PRU-Support@eurocontrol.int","NSA-PRU-Support@eurocontrol.int")</f>
         <v>NSA-PRU-Support@eurocontrol.int</v>
       </c>
@@ -649,59 +674,59 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="6"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="5"/>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="A2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>14</v>
+      <c r="D2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="13">
+      <c r="A3" s="14">
         <v>2017.0</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>19</v>
@@ -726,14 +751,14 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="13">
+      <c r="A4" s="14">
         <v>2017.0</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" s="16">
         <v>7.0</v>
@@ -755,14 +780,14 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="13">
+      <c r="A5" s="14">
         <v>2017.0</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" s="16">
         <v>8.0</v>
@@ -784,14 +809,14 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="13">
+      <c r="A6" s="14">
         <v>2017.0</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D6" s="16">
         <v>8.0</v>
@@ -813,14 +838,14 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="13">
+      <c r="A7" s="14">
         <v>2017.0</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D7" s="16">
         <v>6.0</v>
@@ -842,14 +867,14 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="13">
+      <c r="A8" s="14">
         <v>2017.0</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D8" s="16">
         <v>9.0</v>
@@ -871,14 +896,14 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="13">
+      <c r="A9" s="14">
         <v>2017.0</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D9" s="16">
         <v>9.0</v>
@@ -900,14 +925,14 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="13">
+      <c r="A10" s="14">
         <v>2017.0</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D10" s="16">
         <v>9.0</v>
@@ -929,14 +954,14 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="13">
+      <c r="A11" s="14">
         <v>2017.0</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D11" s="16">
         <v>4.0</v>
@@ -958,14 +983,14 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="13">
+      <c r="A12" s="14">
         <v>2017.0</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12" s="16">
         <v>6.0</v>
@@ -988,42 +1013,42 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C13" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="19" t="s">
+      <c r="I13" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="14">
-      <c r="A14" s="13">
+      <c r="A14" s="14">
         <v>2017.0</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="16">
         <v>5.0</v>
@@ -1045,11 +1070,11 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="13">
+      <c r="A15" s="14">
         <v>2017.0</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>54</v>
@@ -1064,7 +1089,7 @@
         <v>3.0</v>
       </c>
       <c r="G15" s="16">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="H15" s="16">
         <v>1.0</v>
@@ -1074,11 +1099,11 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="13">
+      <c r="A16" s="14">
         <v>2017.0</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>56</v>
@@ -1103,14 +1128,14 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="13">
+      <c r="A17" s="14">
         <v>2017.0</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D17" s="16">
         <v>9.0</v>
@@ -1132,14 +1157,14 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="13">
+      <c r="A18" s="14">
         <v>2017.0</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D18" s="16">
         <v>6.0</v>
@@ -1161,11 +1186,11 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="13">
+      <c r="A19" s="14">
         <v>2017.0</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>65</v>
@@ -1190,14 +1215,14 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="13">
+      <c r="A20" s="14">
         <v>2017.0</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20" s="16">
         <v>7.0</v>
@@ -1219,14 +1244,14 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="13">
+      <c r="A21" s="14">
         <v>2017.0</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D21" s="16">
         <v>4.0</v>
@@ -1248,14 +1273,14 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="13">
+      <c r="A22" s="14">
         <v>2017.0</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D22" s="16">
         <v>6.0</v>
@@ -1277,14 +1302,14 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="13">
+      <c r="A23" s="14">
         <v>2017.0</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D23" s="16">
         <v>7.0</v>
@@ -1306,14 +1331,14 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="13">
+      <c r="A24" s="14">
         <v>2017.0</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D24" s="16">
         <v>9.0</v>
@@ -1336,42 +1361,42 @@
     </row>
     <row r="25">
       <c r="A25" s="17" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E25" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="14">
+        <v>2017.0</v>
+      </c>
+      <c r="B26" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="F25" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="H25" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="I25" s="19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="13">
-        <v>2017.0</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>75</v>
-      </c>
       <c r="C26" s="15" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D26" s="16">
         <v>8.0</v>
@@ -1393,14 +1418,14 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="13">
+      <c r="A27" s="14">
         <v>2017.0</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D27" s="16">
         <v>7.0</v>
@@ -1422,14 +1447,14 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="13">
+      <c r="A28" s="14">
         <v>2017.0</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D28" s="16">
         <v>8.0</v>
@@ -1451,14 +1476,14 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="13">
+      <c r="A29" s="14">
         <v>2017.0</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D29" s="16">
         <v>6.0</v>
@@ -1480,14 +1505,14 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="13">
+      <c r="A30" s="14">
         <v>2017.0</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D30" s="16">
         <v>9.0</v>
@@ -1509,14 +1534,14 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="13">
+      <c r="A31" s="14">
         <v>2017.0</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D31" s="16">
         <v>9.0</v>
@@ -1538,14 +1563,14 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="13">
+      <c r="A32" s="14">
         <v>2017.0</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D32" s="16">
         <v>9.0</v>
@@ -1600,58 +1625,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
+      <c r="C1" s="5"/>
       <c r="D1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6"/>
+      <c r="E1" s="5"/>
       <c r="F1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="6"/>
+        <v>8</v>
+      </c>
+      <c r="G1" s="5"/>
       <c r="H1" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="6"/>
+        <v>9</v>
+      </c>
+      <c r="I1" s="5"/>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="A2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>14</v>
+      <c r="E2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="13">
+      <c r="A3" s="14">
         <v>2017.0</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>18</v>
@@ -1676,11 +1701,11 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="13">
+      <c r="A4" s="14">
         <v>2017.0</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>20</v>
@@ -1705,14 +1730,14 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="13">
+      <c r="A5" s="14">
         <v>2017.0</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="16">
         <v>11.0</v>
@@ -1734,14 +1759,14 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="13">
+      <c r="A6" s="14">
         <v>2017.0</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="16">
         <v>12.0</v>
@@ -1763,20 +1788,20 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="13">
+      <c r="A7" s="14">
         <v>2017.0</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D7" s="16">
         <v>11.0</v>
       </c>
       <c r="E7" s="16">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="F7" s="16">
         <v>2.0</v>
@@ -1792,14 +1817,14 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="13">
+      <c r="A8" s="14">
         <v>2017.0</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D8" s="16">
         <v>12.0</v>
@@ -1821,14 +1846,14 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="13">
+      <c r="A9" s="14">
         <v>2017.0</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D9" s="16">
         <v>13.0</v>
@@ -1850,14 +1875,14 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="13">
+      <c r="A10" s="14">
         <v>2017.0</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" s="16">
         <v>11.0</v>
@@ -1879,14 +1904,14 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="13">
+      <c r="A11" s="14">
         <v>2017.0</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D11" s="16">
         <v>9.0</v>
@@ -1908,14 +1933,14 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="13">
+      <c r="A12" s="14">
         <v>2017.0</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D12" s="16">
         <v>11.0</v>
@@ -1938,42 +1963,42 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D13" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="14">
+        <v>2017.0</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="13">
-        <v>2017.0</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>38</v>
-      </c>
       <c r="C14" s="15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" s="16">
         <v>13.0</v>
@@ -1995,11 +2020,11 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="13">
+      <c r="A15" s="14">
         <v>2017.0</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>55</v>
@@ -2024,11 +2049,11 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="13">
+      <c r="A16" s="14">
         <v>2017.0</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>57</v>
@@ -2053,11 +2078,11 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="13">
+      <c r="A17" s="14">
         <v>2017.0</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>58</v>
@@ -2082,11 +2107,11 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="13">
+      <c r="A18" s="14">
         <v>2017.0</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>59</v>
@@ -2111,14 +2136,14 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="13">
+      <c r="A19" s="14">
         <v>2017.0</v>
       </c>
       <c r="B19" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>61</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>62</v>
       </c>
       <c r="D19" s="16">
         <v>12.0</v>
@@ -2140,14 +2165,14 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="13">
+      <c r="A20" s="14">
         <v>2017.0</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D20" s="16">
         <v>10.0</v>
@@ -2169,14 +2194,14 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="13">
+      <c r="A21" s="14">
         <v>2017.0</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D21" s="16">
         <v>13.0</v>
@@ -2198,14 +2223,14 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="13">
+      <c r="A22" s="14">
         <v>2017.0</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D22" s="16">
         <v>11.0</v>
@@ -2227,14 +2252,14 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="13">
+      <c r="A23" s="14">
         <v>2017.0</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D23" s="16">
         <v>10.0</v>
@@ -2256,14 +2281,14 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="13">
+      <c r="A24" s="14">
         <v>2017.0</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D24" s="16">
         <v>8.0</v>
@@ -2286,39 +2311,39 @@
     </row>
     <row r="25">
       <c r="A25" s="17" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F25" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="I25" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="H25" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" s="19" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="26">
-      <c r="A26" s="13">
+      <c r="A26" s="14">
         <v>2017.0</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>82</v>
@@ -2343,14 +2368,14 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="13">
+      <c r="A27" s="14">
         <v>2017.0</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D27" s="16">
         <v>13.0</v>
@@ -2372,14 +2397,14 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="13">
+      <c r="A28" s="14">
         <v>2017.0</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>84</v>
+        <v>77</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>86</v>
       </c>
       <c r="D28" s="16">
         <v>12.0</v>
@@ -2401,14 +2426,14 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="13">
+      <c r="A29" s="14">
         <v>2017.0</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D29" s="16">
         <v>12.0</v>
@@ -2430,14 +2455,14 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="13">
+      <c r="A30" s="14">
         <v>2017.0</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D30" s="16">
         <v>13.0</v>
@@ -2459,14 +2484,14 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="13">
+      <c r="A31" s="14">
         <v>2017.0</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D31" s="16">
         <v>9.0</v>
@@ -2488,14 +2513,14 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="13">
+      <c r="A32" s="14">
         <v>2017.0</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D32" s="16">
         <v>13.0</v>
@@ -2517,14 +2542,14 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="13">
+      <c r="A33" s="14">
         <v>2017.0</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D33" s="16">
         <v>12.0</v>
@@ -2573,36 +2598,44 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="D1" s="21" t="s">
+      <c r="A1" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" ht="12.75" customHeight="1">
+      <c r="A2" s="9">
+        <v>43311.0</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="24">
+        <v>2017.0</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="26"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>